<commit_message>
Add DDT and pass/fail info. Not work in suite mode.
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="525" windowWidth="24090" windowHeight="11700"/>
+    <workbookView windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
   </bookViews>
   <sheets>
-    <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="13">
   <si>
     <t>Test case name</t>
   </si>
@@ -35,12 +35,31 @@
   </si>
   <si>
     <t>Register with valid credentials_1</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mailTest</t>
+  </si>
+  <si>
+    <t>Register with invalid email_2</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -100,21 +119,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -128,10 +156,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -289,7 +317,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -298,13 +326,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -314,7 +342,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -323,7 +351,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -332,7 +360,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -342,12 +370,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -378,7 +406,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -397,7 +425,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -409,20 +437,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="5" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="42.5703125" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" style="6" width="22.42578125" collapsed="true"/>
+    <col min="7" max="7" style="6" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -430,270 +459,362 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5">
         <v>123456</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="5">
         <v>123456</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>123456</v>
+      </c>
+      <c r="E3" s="5">
+        <v>123456</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add ChooseDriver util class and relative paths of drivers
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="525" windowWidth="24090" windowHeight="11700" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
   </bookViews>
   <sheets>
-    <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
+    <sheet name="LoginData" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>Test case name</t>
   </si>
@@ -99,6 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -164,35 +165,35 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -206,10 +207,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -367,7 +368,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -376,13 +377,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -392,7 +393,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -401,7 +402,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -410,7 +411,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -420,12 +421,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -456,7 +457,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -475,7 +476,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -487,27 +488,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" style="6" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="72.85546875" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="72.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="6" width="22.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -528,7 +529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -549,7 +550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -570,7 +571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -593,7 +594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -612,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -631,7 +632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -640,7 +641,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -649,7 +650,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -658,7 +659,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -667,7 +668,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -676,7 +677,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -685,7 +686,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -694,7 +695,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -703,7 +704,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -712,7 +713,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -721,7 +722,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -730,7 +731,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -739,7 +740,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -748,7 +749,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -757,7 +758,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -766,7 +767,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -775,7 +776,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -784,7 +785,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -793,7 +794,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -802,7 +803,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -811,7 +812,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -820,7 +821,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -829,7 +830,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -838,7 +839,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -847,7 +848,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -856,7 +857,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -865,7 +866,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -874,7 +875,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -883,7 +884,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -892,7 +893,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -901,7 +902,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -912,16 +913,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="F3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -929,14 +930,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="45.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="40.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="45.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -994,10 +995,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink r:id="rId2" ref="B4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add actual behavior on DDT table
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -4,21 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
+    <workbookView xWindow="510" yWindow="525" windowWidth="24090" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
-    <sheet name="LoginData" r:id="rId2" sheetId="2"/>
+    <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
-  <si>
-    <t>Test case name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -62,9 +59,6 @@
     <t>Register with mismatch confirm password_4</t>
   </si>
   <si>
-    <t>Assert massage expected</t>
-  </si>
-  <si>
     <t>You have successfully signed up! Now you should be able to log in.</t>
   </si>
   <si>
@@ -93,13 +87,33 @@
   </si>
   <si>
     <t>Login with invalid email_27_testRedirect</t>
+  </si>
+  <si>
+    <t>Login with invalid password_28</t>
+  </si>
+  <si>
+    <t>Login with invalid password_28_testRedirect</t>
+  </si>
+  <si>
+    <t>Check the form for errors.</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Assert behavior expected</t>
+  </si>
+  <si>
+    <t>Assert behavior actual</t>
+  </si>
+  <si>
+    <t>http://localhost:4200/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -126,7 +140,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +153,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -163,37 +183,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -207,10 +262,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -368,7 +423,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -377,13 +432,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -393,7 +448,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -402,7 +457,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -411,7 +466,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -421,12 +476,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -457,7 +512,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -476,7 +531,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -488,53 +543,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="13.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="6" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="6" width="17.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="6" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="72.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="6" width="22.42578125" collapsed="true"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" style="6" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="59.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="50.7109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.28515625" style="10" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5">
@@ -544,18 +605,21 @@
         <v>123456</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5">
@@ -565,21 +629,24 @@
         <v>123456</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5">
         <v>123456</v>
@@ -588,18 +655,21 @@
         <v>123456</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5">
@@ -608,397 +678,485 @@
       <c r="E5" s="5">
         <v>1234</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5">
         <v>12345</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="8"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="8"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" s="8"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" s="8"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="8"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="8"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="8"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="8"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="8"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="8"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="8"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="8"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="8"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="8"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="8"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="8"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="8"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="8"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="8"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="8"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="8"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="8"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="8"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="8"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="8"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="8"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="8"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="8"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="8"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="8"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink ref="F3" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="5" width="45.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="40.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="45.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="26.7109375" collapsed="true"/>
+    <col min="1" max="1" width="45.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="45.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.7109375" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
-    <hyperlink r:id="rId2" ref="B4"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add BasePage and AddNewFlowerPage
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="525" windowWidth="24090" windowHeight="11700" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
   </bookViews>
   <sheets>
-    <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
+    <sheet name="LoginData" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -114,6 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -207,48 +208,48 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -262,10 +263,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -423,7 +424,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -432,13 +433,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -448,7 +449,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -457,7 +458,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -466,7 +467,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -476,12 +477,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -512,7 +513,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -531,7 +532,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -543,27 +544,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" style="6" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="59.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="50.7109375" style="6" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22.42578125" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.28515625" style="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="6" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="59.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="6" width="58.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="11.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="10" width="30.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -590,7 +591,7 @@
       </c>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -614,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -638,7 +639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -664,7 +665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -688,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -712,7 +713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -722,7 +723,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -732,7 +733,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -742,7 +743,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -752,7 +753,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -762,7 +763,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -772,7 +773,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -782,7 +783,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -792,7 +793,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -802,7 +803,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -812,7 +813,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -822,7 +823,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -832,7 +833,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -842,7 +843,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -852,7 +853,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -862,7 +863,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -872,7 +873,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -882,7 +883,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -892,7 +893,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -902,7 +903,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -912,7 +913,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -922,7 +923,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -932,7 +933,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -942,7 +943,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -952,7 +953,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -962,7 +963,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -972,7 +973,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -982,7 +983,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -992,7 +993,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1002,7 +1003,7 @@
       <c r="G35" s="8"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1012,7 +1013,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1024,31 +1025,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="F3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="45.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="45.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="15.5703125" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="5" width="45.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15.75" r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15" r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="15" r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1152,11 +1153,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink r:id="rId2" ref="B4"/>
+    <hyperlink r:id="rId3" ref="D4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add screenshot after each test
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>AssertFalse()</t>
+  </si>
+  <si>
+    <t>E-mail already exists!</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1339,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
start test home page
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
+    <workbookView activeTab="2" windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="50">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
   <si>
     <t>password</t>
   </si>
@@ -111,9 +108,6 @@
     <t>http://localhost:4200/</t>
   </si>
   <si>
-    <t>Case action</t>
-  </si>
-  <si>
     <t>Flower name</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>http://localhost:4200/flowers/details/</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -165,7 +156,13 @@
     <t>AssertFalse()</t>
   </si>
   <si>
-    <t>E-mail already exists!</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Test case name</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
   </si>
 </sst>
 </file>
@@ -263,7 +260,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
@@ -305,6 +302,18 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -610,9 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -621,7 +628,7 @@
     <col min="3" max="3" customWidth="true" style="6" width="12.42578125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="6" width="17.140625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="6" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="59.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="19" width="59.42578125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="6" width="58.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="11.42578125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="5" width="25.85546875" collapsed="true"/>
@@ -629,39 +636,39 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5">
@@ -670,22 +677,22 @@
       <c r="E2" s="5">
         <v>123456</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
+      <c r="F2" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5">
@@ -694,25 +701,25 @@
       <c r="E3" s="5">
         <v>123456</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>16</v>
+      <c r="F3" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5">
         <v>123456</v>
@@ -720,22 +727,22 @@
       <c r="E4" s="5">
         <v>123456</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
+      <c r="F4" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5">
@@ -744,44 +751,44 @@
       <c r="E5" s="5">
         <v>1234</v>
       </c>
-      <c r="F5" s="5" t="b">
+      <c r="F5" s="16" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5">
         <v>12345</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="F6" s="5" t="b">
+      <c r="F6" s="16" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -790,7 +797,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
@@ -800,7 +807,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
@@ -810,7 +817,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
@@ -820,7 +827,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="8"/>
       <c r="H10" s="5"/>
     </row>
@@ -830,7 +837,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
@@ -840,7 +847,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
@@ -850,7 +857,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="8"/>
       <c r="H13" s="5"/>
     </row>
@@ -860,7 +867,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
@@ -870,7 +877,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
@@ -880,7 +887,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
@@ -890,7 +897,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="16"/>
       <c r="G17" s="8"/>
       <c r="H17" s="5"/>
     </row>
@@ -900,7 +907,7 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="8"/>
       <c r="H18" s="5"/>
     </row>
@@ -910,7 +917,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
@@ -920,7 +927,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="8"/>
       <c r="H20" s="5"/>
     </row>
@@ -930,7 +937,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="16"/>
       <c r="G21" s="8"/>
       <c r="H21" s="5"/>
     </row>
@@ -940,7 +947,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="8"/>
       <c r="H22" s="5"/>
     </row>
@@ -950,7 +957,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
@@ -960,7 +967,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="8"/>
       <c r="H24" s="5"/>
     </row>
@@ -970,7 +977,7 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="8"/>
       <c r="H25" s="5"/>
     </row>
@@ -980,7 +987,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="8"/>
       <c r="H26" s="5"/>
     </row>
@@ -990,7 +997,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="8"/>
       <c r="H27" s="5"/>
     </row>
@@ -1000,7 +1007,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="8"/>
       <c r="H28" s="5"/>
     </row>
@@ -1010,7 +1017,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="8"/>
       <c r="H29" s="5"/>
     </row>
@@ -1020,7 +1027,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="8"/>
       <c r="H30" s="5"/>
     </row>
@@ -1030,7 +1037,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="8"/>
       <c r="H31" s="5"/>
     </row>
@@ -1040,7 +1047,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="8"/>
       <c r="H32" s="5"/>
     </row>
@@ -1050,7 +1057,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="8"/>
       <c r="H33" s="5"/>
     </row>
@@ -1060,7 +1067,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="8"/>
       <c r="H34" s="5"/>
     </row>
@@ -1070,7 +1077,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="16"/>
       <c r="G35" s="8"/>
       <c r="H35" s="5"/>
     </row>
@@ -1080,7 +1087,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="16"/>
       <c r="G36" s="8"/>
       <c r="H36" s="5"/>
     </row>
@@ -1090,7 +1097,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="F37" s="16"/>
       <c r="G37" s="8"/>
       <c r="H37" s="5"/>
     </row>
@@ -1107,9 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1122,104 +1127,104 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row customHeight="1" ht="15" r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>18</v>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row customHeight="1" ht="15" r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1237,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K894"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1257,95 +1262,95 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>37</v>
-      </c>
       <c r="B2" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="11">
         <v>100</v>
       </c>
       <c r="F2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>43</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="11">
         <v>100</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
work on home page
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
   <si>
     <t>password</t>
   </si>
@@ -1127,7 +1127,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
finish first home page test
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -10,13 +10,14 @@
     <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
     <sheet name="LoginData" r:id="rId2" sheetId="2"/>
     <sheet name="AddNewFlowerData" r:id="rId3" sheetId="3"/>
+    <sheet name="AddNewFlowerForTestHomePage" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>password</t>
   </si>
@@ -160,6 +161,33 @@
   </si>
   <si>
     <t>Test case name</t>
+  </si>
+  <si>
+    <t>TestRose</t>
+  </si>
+  <si>
+    <t>Rosses</t>
+  </si>
+  <si>
+    <t>http://www.mmtrbg.com/uploads/com_article/gallery/c5664e01e57f4edb2b69a47edd313d614dd4b3f3.jpg</t>
+  </si>
+  <si>
+    <t>Check correct added flower_55</t>
+  </si>
+  <si>
+    <t>First username</t>
+  </si>
+  <si>
+    <t>Second username</t>
+  </si>
+  <si>
+    <t>firstTestUser</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>AssertTrue()</t>
   </si>
   <si>
     <t>SKIPPED</t>
@@ -619,7 +647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1127,7 +1157,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -1242,9 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K894"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1262,7 +1290,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>30</v>
@@ -11163,4 +11191,105 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" customWidth="true" style="5" width="29.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="28.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="5" width="22.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="5" width="89.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="5" width="25.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="24.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="27.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="5" width="23.5703125" collapsed="true"/>
+    <col min="13" max="14" style="6" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="5">
+        <v>100</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add buy flower test
</commit_message>
<xml_diff>
--- a/ui.tests/src/test/java/resources/testData.xlsx
+++ b/ui.tests/src/test/java/resources/testData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
+    <workbookView activeTab="4" windowHeight="11700" windowWidth="24090" xWindow="510" yWindow="525"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterData" r:id="rId1" sheetId="1"/>
     <sheet name="LoginData" r:id="rId2" sheetId="2"/>
     <sheet name="AddNewFlowerData" r:id="rId3" sheetId="3"/>
     <sheet name="AddNewFlowerForTestHomePage" r:id="rId4" sheetId="4"/>
+    <sheet name="BuyFlowerData" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
   <si>
     <t>password</t>
   </si>
@@ -192,6 +193,42 @@
   <si>
     <t>SKIPPED</t>
   </si>
+  <si>
+    <t>Buy flower</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/MZICbG7YniA/hqdefault.jpg</t>
+  </si>
+  <si>
+    <t>Snowdrop</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>secondTestUser</t>
+  </si>
+  <si>
+    <t>Order address</t>
+  </si>
+  <si>
+    <t>test address</t>
+  </si>
+  <si>
+    <t>Payment method</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Order email</t>
+  </si>
+  <si>
+    <t>test@email.eu</t>
+  </si>
+  <si>
+    <t>Thank you for your purchase! We will contact you soon at test@email.eu!</t>
+  </si>
 </sst>
 </file>
 
@@ -224,7 +261,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,7 +331,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
@@ -341,6 +384,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1272,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K894"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11198,7 +11251,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11291,5 +11344,138 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="21" width="29.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="21" width="30.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="21" width="27.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="21" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="21" width="9.85546875" collapsed="true"/>
+    <col min="6" max="7" style="21" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="21" width="42.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="21" width="42.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="21" width="42.7109375" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="21" width="42.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="21" width="63.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="20" width="63.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="21" width="8.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="21" width="11.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="20">
+        <v>100</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="20"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="H2"/>
+    <hyperlink r:id="rId2" ref="J2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>